<commit_message>
final touches. pretty much fully functional
</commit_message>
<xml_diff>
--- a/dokumentasjon/Teknisk Dokumentasjon.xlsx
+++ b/dokumentasjon/Teknisk Dokumentasjon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeoslokommuneno-my.sharepoint.com/personal/jomaa058_osloskolen_no/Documents/Project Management/Årsoppgave/dokumentasjon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeoslokommuneno-my.sharepoint.com/personal/jomaa058_osloskolen_no/Documents/Project Management/Årsoppgave/programkode/battleship/dokumentasjon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{5153BE53-1359-418D-AD6B-2A9D3505250C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9837ABEE-EE9E-4056-8E24-12D49CFAEBDE}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8_{5153BE53-1359-418D-AD6B-2A9D3505250C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1E682CB-FDCA-4360-8CAC-27A01E729CE6}"/>
   <bookViews>
-    <workbookView xWindow="9615" yWindow="-14070" windowWidth="17160" windowHeight="12300" xr2:uid="{3E2B356F-88BD-440C-98B6-C3DB7E0857E9}"/>
+    <workbookView xWindow="9528" yWindow="120" windowWidth="13512" windowHeight="12240" xr2:uid="{3E2B356F-88BD-440C-98B6-C3DB7E0857E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Maskinnavn</t>
   </si>
@@ -71,9 +71,6 @@
     <t>sudo mysql -u root -p</t>
   </si>
   <si>
-    <t>djatabase</t>
-  </si>
-  <si>
     <t>root</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>php myadmin</t>
   </si>
   <si>
-    <t>sammy</t>
-  </si>
-  <si>
     <t>MYSQL</t>
   </si>
   <si>
@@ -107,7 +101,7 @@
     <t>SERVER @</t>
   </si>
   <si>
-    <t>DATABASE @</t>
+    <t>DjATABASE @</t>
   </si>
 </sst>
 </file>
@@ -180,6 +174,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -482,7 +480,7 @@
   <dimension ref="B2:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,10 +491,10 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
@@ -533,54 +531,44 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>11</v>
       </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
-        <v>7</v>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
@@ -601,15 +589,15 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
         <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" xr:uid="{64BD1D97-2A55-4F17-BEB8-35D70DFBFA02}"/>
+    <hyperlink ref="C10" r:id="rId1" xr:uid="{64BD1D97-2A55-4F17-BEB8-35D70DFBFA02}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
save game plus tekniske dokumenter
</commit_message>
<xml_diff>
--- a/dokumentasjon/Teknisk Dokumentasjon.xlsx
+++ b/dokumentasjon/Teknisk Dokumentasjon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeoslokommuneno-my.sharepoint.com/personal/jomaa058_osloskolen_no/Documents/Project Management/Årsoppgave/programkode/battleship/dokumentasjon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive - Osloskolen\Project Management\Årsoppgave\programkode\battleship\dokumentasjon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="8_{5153BE53-1359-418D-AD6B-2A9D3505250C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1E682CB-FDCA-4360-8CAC-27A01E729CE6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34E8F97-2C60-433B-90F8-C082A917DF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9528" yWindow="120" windowWidth="13512" windowHeight="12240" xr2:uid="{3E2B356F-88BD-440C-98B6-C3DB7E0857E9}"/>
+    <workbookView xWindow="21510" yWindow="345" windowWidth="16890" windowHeight="15300" xr2:uid="{3E2B356F-88BD-440C-98B6-C3DB7E0857E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Maskinnavn</t>
   </si>
@@ -89,9 +89,6 @@
     <t>php myadmin</t>
   </si>
   <si>
-    <t>MYSQL</t>
-  </si>
-  <si>
     <t>10.2.2.146</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>DjATABASE @</t>
+  </si>
+  <si>
+    <t>MYSQL @</t>
   </si>
 </sst>
 </file>
@@ -174,10 +174,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -477,27 +473,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137E27AA-D6D8-457F-923A-B0E6F6A3FBDF}">
-  <dimension ref="B2:C19"/>
+  <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -505,7 +501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -513,7 +509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -521,7 +517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -529,15 +525,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -545,7 +541,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -553,12 +549,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -566,32 +562,35 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>